<commit_message>
land use change is not summing up properly
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\drawing_figures\gcam-sandbox\input\gcamdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\ManurePyrolysisIAM\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CEEA33-C5AD-4698-8600-EC853EB970A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BB9963-779B-4828-A10A-CA684D0F9F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="983" yWindow="-98" windowWidth="27915" windowHeight="16395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyrolysis-nofert" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>hrs/day</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>(4 years from 2024)</t>
+  </si>
+  <si>
+    <t>Sequestered C Ratio (Mg C/Mg Manure)</t>
   </si>
 </sst>
 </file>
@@ -512,16 +515,16 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>3</v>
       </c>
@@ -529,7 +532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>24</v>
       </c>
@@ -537,7 +540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>330</v>
       </c>
@@ -548,7 +551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.31819999999999998</v>
       </c>
@@ -559,7 +562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>0.35</v>
       </c>
@@ -570,7 +573,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>0.35</v>
       </c>
@@ -581,7 +584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>0.35</v>
       </c>
@@ -592,7 +595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>0.26</v>
       </c>
@@ -603,7 +606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3.8999999999999998E-3</v>
       </c>
@@ -614,7 +617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>1000</v>
       </c>
@@ -622,10 +625,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -633,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -662,7 +665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -703,7 +706,7 @@
         <v>805.8147593031315</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -744,7 +747,7 @@
         <v>732.60073260073261</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -785,7 +788,7 @@
         <v>732.60073260073261</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -826,7 +829,7 @@
         <v>732.60073260073261</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -867,12 +870,12 @@
         <v>986.19329388560163</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -889,7 +892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -907,7 +910,7 @@
         <v>30.425531914893618</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -925,7 +928,7 @@
         <v>58.111111111111114</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -943,7 +946,7 @@
         <v>27.312925170068027</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -961,7 +964,7 @@
         <v>27.312925170068027</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -980,20 +983,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C229AC-139E-41F1-AA79-F61EE8EC5D09}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>3</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>24</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>330</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <f>1/2.1815</f>
         <v>0.45840018336007332</v>
@@ -1032,7 +1035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <f>1/2.1052</f>
         <v>0.47501425042751283</v>
@@ -1044,7 +1047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f>1/2.055</f>
         <v>0.48661800486618001</v>
@@ -1056,7 +1059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f>1/2.136</f>
         <v>0.46816479400749061</v>
@@ -1068,7 +1071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <f>1/2.1276</f>
         <v>0.47001316036849028</v>
@@ -1080,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>1000</v>
       </c>
@@ -1088,10 +1091,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1159,7 @@
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1193,7 @@
       </c>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1224,7 +1227,7 @@
       </c>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1261,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1292,12 +1295,12 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -1310,11 +1313,14 @@
       <c r="E20" t="s">
         <v>33</v>
       </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
       <c r="G20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1331,8 +1337,12 @@
         <f>(B21+C21)/(D21*1000000)</f>
         <v>30.425531914893618</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="3">
+        <f>(C21)/(D21*1000000*100)</f>
+        <v>0.13085106382978723</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1349,8 +1359,12 @@
         <f t="shared" ref="E22:E24" si="0">(B22+C22)/(D22*1000000)</f>
         <v>58.111111111111114</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="3">
+        <f t="shared" ref="F22:F24" si="1">(C22)/(D22*1000000*100)</f>
+        <v>0.14301587301587301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1367,8 +1381,12 @@
         <f t="shared" si="0"/>
         <v>27.312925170068027</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11326530612244898</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1385,8 +1403,12 @@
         <f t="shared" si="0"/>
         <v>27.312925170068027</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>0.11326530612244898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1405,13 +1427,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248186C2-819E-40A3-BDA6-AECDD5B5B57C}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>39</v>
       </c>
@@ -1485,7 +1507,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="E2" t="s">
         <v>45</v>
       </c>
@@ -1550,7 +1572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1643,7 +1665,7 @@
         <v>2.5889995662654433</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1736,7 +1758,7 @@
         <v>0.45359192400983966</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1851,7 @@
         <v>3.1009994804902044</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1922,7 +1944,7 @@
         <v>0.30399994907095201</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2015,19 +2037,19 @@
         <v>1.3809997686413971</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G9">
         <f>-$C3*EXP(-$D3*G$1-$E3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G10">
         <f>EXP(-$D3*G$1-$E3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G11">
         <f>-$D3*G$1-$E3</f>
         <v>-2521.75</v>

</xml_diff>

<commit_message>
nutrient application rate parameters updated
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\ManurePyrolysisIAM\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BB9963-779B-4828-A10A-CA684D0F9F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1DF9DD-C05F-43F0-B53B-6726988F7BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="983" yWindow="-98" windowWidth="27915" windowHeight="16395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1148" yWindow="60" windowWidth="20790" windowHeight="8475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyrolysis-nofert" sheetId="1" r:id="rId1"/>
@@ -185,10 +185,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -219,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -229,6 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C229AC-139E-41F1-AA79-F61EE8EC5D09}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1311,7 +1313,7 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
         <v>46</v>
@@ -1333,11 +1335,11 @@
       <c r="D21">
         <v>94</v>
       </c>
-      <c r="E21" s="7">
-        <f>(B21+C21)/(D21*1000000)</f>
-        <v>30.425531914893618</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E21" s="9">
+        <f>(B21)/(D21*1000000*100)</f>
+        <v>0.17340425531914894</v>
+      </c>
+      <c r="F21" s="9">
         <f>(C21)/(D21*1000000*100)</f>
         <v>0.13085106382978723</v>
       </c>
@@ -1355,11 +1357,11 @@
       <c r="D22">
         <v>63</v>
       </c>
-      <c r="E22" s="7">
-        <f t="shared" ref="E22:E24" si="0">(B22+C22)/(D22*1000000)</f>
-        <v>58.111111111111114</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="E22" s="9">
+        <f t="shared" ref="E22:E25" si="0">(B22)/(D22*1000000*100)</f>
+        <v>0.43809523809523809</v>
+      </c>
+      <c r="F22" s="9">
         <f t="shared" ref="F22:F24" si="1">(C22)/(D22*1000000*100)</f>
         <v>0.14301587301587301</v>
       </c>
@@ -1377,11 +1379,11 @@
       <c r="D23">
         <v>294</v>
       </c>
-      <c r="E23" s="7">
-        <f t="shared" si="0"/>
-        <v>27.312925170068027</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="E23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1598639455782313</v>
+      </c>
+      <c r="F23" s="9">
         <f t="shared" si="1"/>
         <v>0.11326530612244898</v>
       </c>
@@ -1399,11 +1401,11 @@
       <c r="D24">
         <v>294</v>
       </c>
-      <c r="E24" s="7">
-        <f t="shared" si="0"/>
-        <v>27.312925170068027</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="E24" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1598639455782313</v>
+      </c>
+      <c r="F24" s="9">
         <f t="shared" si="1"/>
         <v>0.11326530612244898</v>
       </c>
@@ -1415,7 +1417,10 @@
       <c r="B25" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
non-energy costs are per unit input
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25F245-6920-4EFF-B232-E03D709A6076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421749A2-B851-4DF0-9F25-9FA2E26AC9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>Poultry</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Lima, I. M., McAloon, A. &amp; Boateng, A. A. Activated carbon from broiler litter: Process description and cost of production. Biomass and Bioenergy 32, 568â572 (2008).</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
   </si>
   <si>
     <t>same as beef/dairy</t>
-  </si>
-  <si>
-    <t>Unit cost  ($1975/kg)</t>
   </si>
   <si>
     <t>B_max</t>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>Production estimates (kg per year)</t>
+  </si>
+  <si>
+    <t>Unit cost  ($1975/kg input)</t>
+  </si>
+  <si>
+    <t>manure</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,15 +583,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,10 +599,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,10 +610,10 @@
         <v>0.8</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,10 +621,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,10 +632,10 @@
         <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,10 +651,10 @@
         <v>3600000</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>10600000</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>0.26</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>0.12</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>0.09</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -701,10 +701,10 @@
         <v>0.45840018336007332</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,10 +713,10 @@
         <v>0.47501425042751283</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,10 +725,10 @@
         <v>0.48661800486618001</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,10 +737,10 @@
         <v>0.46816479400749061</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -749,10 +749,10 @@
         <v>0.47001316036849028</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -780,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -938,27 +938,51 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" ref="B27" si="5">(A$8+A$9)*A$10</f>
+        <v>3692000</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" ref="C27" si="6">0.09*B27</f>
+        <v>332280</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ref="D27" si="7">-PV(A$11,A$5,C27)+B27</f>
+        <v>6173946.7274915744</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" ref="E27" si="8">-PMT(A$11,A$5,D27)</f>
+        <v>826560.45590642723</v>
+      </c>
+      <c r="F27">
+        <f>A$3*A$4*A$6*A$7*A$18</f>
+        <v>70080000</v>
+      </c>
+      <c r="G27" s="5">
+        <f>E27/F27</f>
+        <v>1.1794527053459293E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>24</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
         <v>25</v>
-      </c>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -997,11 +1021,11 @@
         <v>63</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" ref="E31:E34" si="5">(B31)/(D31*1000000*100)</f>
+        <f t="shared" ref="E31:E34" si="9">(B31)/(D31*1000000*100)</f>
         <v>0.43809523809523809</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" ref="F31:F33" si="6">(C31)/(D31*1000000*100)</f>
+        <f t="shared" ref="F31:F33" si="10">(C31)/(D31*1000000*100)</f>
         <v>0.14301587301587301</v>
       </c>
     </row>
@@ -1019,11 +1043,11 @@
         <v>294</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1041,11 +1065,11 @@
         <v>294</v>
       </c>
       <c r="E33" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1054,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="3" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1079,19 +1103,19 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
       <c r="G1">
         <v>1975</v>
@@ -1153,10 +1177,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2">
         <v>0</v>

</xml_diff>

<commit_message>
check first model output
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421749A2-B851-4DF0-9F25-9FA2E26AC9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE40A35-7B97-4C88-9F5C-660A6E8026FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,21 +90,6 @@
     <t>tons feedstock/hr</t>
   </si>
   <si>
-    <t>beef biooil yield</t>
-  </si>
-  <si>
-    <t>dairy biooil yield</t>
-  </si>
-  <si>
-    <t>goat biooil yield</t>
-  </si>
-  <si>
-    <t>pork biooil yield</t>
-  </si>
-  <si>
-    <t>poultry biooil yield</t>
-  </si>
-  <si>
     <t>Avoided C</t>
   </si>
   <si>
@@ -206,13 +191,28 @@
     <t>interest rate</t>
   </si>
   <si>
-    <t>Production estimates (kg per year)</t>
-  </si>
-  <si>
-    <t>Unit cost  ($1975/kg input)</t>
-  </si>
-  <si>
     <t>manure</t>
+  </si>
+  <si>
+    <t>Production estimates (kg biochar per year)</t>
+  </si>
+  <si>
+    <t>Unit cost  ($1975/kg biochar)</t>
+  </si>
+  <si>
+    <t>beef biochar yield</t>
+  </si>
+  <si>
+    <t>goat biochar yield</t>
+  </si>
+  <si>
+    <t>pork biochar yield</t>
+  </si>
+  <si>
+    <t>poultry biochar yield</t>
+  </si>
+  <si>
+    <t>dairy biochar yield</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,15 +583,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,10 +610,10 @@
         <v>0.8</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,10 +621,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -643,7 +643,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,10 +651,10 @@
         <v>3600000</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>10600000</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>0.26</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>0.12</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>0.09</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -701,7 +701,7 @@
         <v>0.45840018336007332</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -713,7 +713,7 @@
         <v>0.47501425042751283</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -725,7 +725,7 @@
         <v>0.48661800486618001</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -737,7 +737,7 @@
         <v>0.46816479400749061</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -749,7 +749,7 @@
         <v>0.47001316036849028</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -780,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>32124684.849873938</v>
       </c>
       <c r="G22" s="5">
-        <f>E22/F22</f>
+        <f t="shared" ref="G22:G27" si="0">E22/F22</f>
         <v>2.5729760767121451E-2</v>
       </c>
       <c r="I22" s="8"/>
@@ -821,15 +821,15 @@
         <v>7</v>
       </c>
       <c r="B23" s="10">
-        <f t="shared" ref="B23:B26" si="0">(A$8+A$9)*A$10</f>
+        <f t="shared" ref="B23:B26" si="1">(A$8+A$9)*A$10</f>
         <v>3692000</v>
       </c>
       <c r="C23" s="10">
-        <f t="shared" ref="C23:C26" si="1">0.09*B23</f>
+        <f t="shared" ref="C23:C26" si="2">0.09*B23</f>
         <v>332280</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" ref="D23:D26" si="2">-PV(A$11,A$5,C23)+B23</f>
+        <f t="shared" ref="D23:D26" si="3">-PV(A$11,A$5,C23)+B23</f>
         <v>6173946.7274915744</v>
       </c>
       <c r="E23" s="4">
@@ -841,7 +841,7 @@
         <v>33288998.6699601</v>
       </c>
       <c r="G23" s="5">
-        <f>E23/F23</f>
+        <f t="shared" si="0"/>
         <v>2.4829838352942502E-2</v>
       </c>
       <c r="I23" s="8"/>
@@ -851,27 +851,27 @@
         <v>8</v>
       </c>
       <c r="B24" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3692000</v>
       </c>
       <c r="C24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>332280</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" ref="E24:E26" si="3">-PMT(A$11,A$5,D24)</f>
+        <f t="shared" ref="E24:E26" si="4">-PMT(A$11,A$5,D24)</f>
         <v>826560.45590642723</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F26" si="4">A$3*A$4*A$6*A$7*A15*A$18</f>
+        <f t="shared" ref="F24:F26" si="5">A$3*A$4*A$6*A$7*A15*A$18</f>
         <v>34102189.781021893</v>
       </c>
       <c r="G24" s="5">
-        <f>E24/F24</f>
+        <f t="shared" si="0"/>
         <v>2.4237753094858851E-2</v>
       </c>
       <c r="I24" s="8"/>
@@ -881,27 +881,27 @@
         <v>9</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3692000</v>
       </c>
       <c r="C25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>332280</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>826560.45590642723</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32808988.764044944</v>
       </c>
       <c r="G25" s="5">
-        <f>E25/F25</f>
+        <f t="shared" si="0"/>
         <v>2.519310978618905E-2</v>
       </c>
       <c r="I25" s="8"/>
@@ -911,49 +911,49 @@
         <v>10</v>
       </c>
       <c r="B26" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3692000</v>
       </c>
       <c r="C26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>332280</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>826560.45590642723</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32938522.278623801</v>
       </c>
       <c r="G26" s="5">
-        <f>E26/F26</f>
+        <f t="shared" si="0"/>
         <v>2.5094035758939991E-2</v>
       </c>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" s="10">
-        <f t="shared" ref="B27" si="5">(A$8+A$9)*A$10</f>
+        <f t="shared" ref="B27" si="6">(A$8+A$9)*A$10</f>
         <v>3692000</v>
       </c>
       <c r="C27" s="10">
-        <f t="shared" ref="C27" si="6">0.09*B27</f>
+        <f t="shared" ref="C27" si="7">0.09*B27</f>
         <v>332280</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27" si="7">-PV(A$11,A$5,C27)+B27</f>
+        <f t="shared" ref="D27" si="8">-PV(A$11,A$5,C27)+B27</f>
         <v>6173946.7274915744</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27" si="8">-PMT(A$11,A$5,D27)</f>
+        <f t="shared" ref="E27" si="9">-PMT(A$11,A$5,D27)</f>
         <v>826560.45590642723</v>
       </c>
       <c r="F27">
@@ -961,28 +961,28 @@
         <v>70080000</v>
       </c>
       <c r="G27" s="5">
-        <f>E27/F27</f>
+        <f t="shared" si="0"/>
         <v>1.1794527053459293E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,11 +1021,11 @@
         <v>63</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" ref="E31:E34" si="9">(B31)/(D31*1000000*100)</f>
+        <f t="shared" ref="E31:E34" si="10">(B31)/(D31*1000000*100)</f>
         <v>0.43809523809523809</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" ref="F31:F33" si="10">(C31)/(D31*1000000*100)</f>
+        <f t="shared" ref="F31:F33" si="11">(C31)/(D31*1000000*100)</f>
         <v>0.14301587301587301</v>
       </c>
     </row>
@@ -1043,11 +1043,11 @@
         <v>294</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1065,11 +1065,11 @@
         <v>294</v>
       </c>
       <c r="E33" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1078,10 +1078,10 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1103,19 +1103,19 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G1">
         <v>1975</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>0</v>

</xml_diff>

<commit_message>
testing biochar unit costs not including capex
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200054FD-E48C-49F9-81CE-67F5B0DA27DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B9AB2-B193-4427-9593-8929AD134FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biochar_land" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>CAPEX</t>
   </si>
@@ -213,6 +213,21 @@
   </si>
   <si>
     <t>dairy biochar yield</t>
+  </si>
+  <si>
+    <t>Only OPEX costs (test for costs by tech)</t>
+  </si>
+  <si>
+    <t>Total Costs</t>
+  </si>
+  <si>
+    <t>To EUAW</t>
+  </si>
+  <si>
+    <t>Production Estimate</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
   </si>
 </sst>
 </file>
@@ -271,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -283,6 +298,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -564,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C229AC-139E-41F1-AA79-F61EE8EC5D09}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +595,9 @@
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -743,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>1/2.1276</f>
         <v>0.47001316036849028</v>
@@ -755,7 +774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1000</v>
       </c>
@@ -763,10 +782,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -785,8 +804,23 @@
       <c r="G21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" t="s">
+        <v>53</v>
+      </c>
+      <c r="O21" t="s">
+        <v>54</v>
+      </c>
+      <c r="P21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -815,21 +849,41 @@
         <v>2.5729760767121451E-2</v>
       </c>
       <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L22" s="11">
+        <f>C22</f>
+        <v>332280</v>
+      </c>
+      <c r="M22" s="4">
+        <f>-PV(A$11,A$5,C22)</f>
+        <v>2481946.7274915739</v>
+      </c>
+      <c r="N22" s="4">
+        <f>-PMT(A$11,A$5,M22)</f>
+        <v>332280.00000000006</v>
+      </c>
+      <c r="O22">
+        <f>F22</f>
+        <v>32124684.849873938</v>
+      </c>
+      <c r="P22" s="5">
+        <f t="shared" ref="P22:P26" si="1">N22/O22</f>
+        <v>1.0343447773972605E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="10">
-        <f t="shared" ref="B23:B26" si="1">(A$8+A$9)*A$10</f>
+        <f t="shared" ref="B23:B26" si="2">(A$8+A$9)*A$10</f>
         <v>3692000</v>
       </c>
       <c r="C23" s="10">
-        <f t="shared" ref="C23:C26" si="2">0.09*B23</f>
+        <f t="shared" ref="C23:C26" si="3">0.09*B23</f>
         <v>332280</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" ref="D23:D26" si="3">-PV(A$11,A$5,C23)+B23</f>
+        <f t="shared" ref="D23:D26" si="4">-PV(A$11,A$5,C23)+B23</f>
         <v>6173946.7274915744</v>
       </c>
       <c r="E23" s="4">
@@ -845,29 +899,49 @@
         <v>2.4829838352942502E-2</v>
       </c>
       <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L23" s="11">
+        <f t="shared" ref="L23:L26" si="5">C23</f>
+        <v>332280</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" ref="M23:M26" si="6">-PV(A$11,A$5,C23)</f>
+        <v>2481946.7274915739</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" ref="N23:N26" si="7">-PMT(A$11,A$5,M23)</f>
+        <v>332280.00000000006</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:O26" si="8">F23</f>
+        <v>33288998.6699601</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="shared" si="1"/>
+        <v>9.9816760273972616E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3692000</v>
       </c>
       <c r="C24" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>332280</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" ref="E24:E26" si="4">-PMT(A$11,A$5,D24)</f>
+        <f t="shared" ref="E24:E26" si="9">-PMT(A$11,A$5,D24)</f>
         <v>826560.45590642723</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F26" si="5">A$3*A$4*A$6*A$7*A15*A$18</f>
+        <f t="shared" ref="F24:F26" si="10">A$3*A$4*A$6*A$7*A15*A$18</f>
         <v>34102189.781021893</v>
       </c>
       <c r="G24" s="5">
@@ -875,85 +949,145 @@
         <v>2.4237753094858851E-2</v>
       </c>
       <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L24" s="11">
+        <f t="shared" si="5"/>
+        <v>332280</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" si="6"/>
+        <v>2481946.7274915739</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="7"/>
+        <v>332280.00000000006</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="8"/>
+        <v>34102189.781021893</v>
+      </c>
+      <c r="P24" s="5">
+        <f t="shared" si="1"/>
+        <v>9.743655821917812E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3692000</v>
       </c>
       <c r="C25" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>332280</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>826560.45590642723</v>
       </c>
       <c r="F25">
+        <f t="shared" si="10"/>
+        <v>32808988.764044944</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>2.519310978618905E-2</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="L25" s="11">
         <f t="shared" si="5"/>
+        <v>332280</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" si="6"/>
+        <v>2481946.7274915739</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="7"/>
+        <v>332280.00000000006</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="8"/>
         <v>32808988.764044944</v>
       </c>
-      <c r="G25" s="5">
-        <f t="shared" si="0"/>
-        <v>2.519310978618905E-2</v>
-      </c>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P25" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0127712328767125E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3692000</v>
       </c>
       <c r="C26" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>332280</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6173946.7274915744</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>826560.45590642723</v>
       </c>
       <c r="F26">
+        <f t="shared" si="10"/>
+        <v>32938522.278623801</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5094035758939991E-2</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="L26" s="11">
         <f t="shared" si="5"/>
+        <v>332280</v>
+      </c>
+      <c r="M26" s="4">
+        <f t="shared" si="6"/>
+        <v>2481946.7274915739</v>
+      </c>
+      <c r="N26" s="4">
+        <f t="shared" si="7"/>
+        <v>332280.00000000006</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="8"/>
         <v>32938522.278623801</v>
       </c>
-      <c r="G26" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5094035758939991E-2</v>
-      </c>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P26" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0087884246575345E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="10">
-        <f t="shared" ref="B27" si="6">(A$8+A$9)*A$10</f>
+        <f t="shared" ref="B27" si="11">(A$8+A$9)*A$10</f>
         <v>3692000</v>
       </c>
       <c r="C27" s="10">
-        <f t="shared" ref="C27" si="7">0.09*B27</f>
+        <f t="shared" ref="C27" si="12">0.09*B27</f>
         <v>332280</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27" si="8">-PV(A$11,A$5,C27)+B27</f>
+        <f t="shared" ref="D27" si="13">-PV(A$11,A$5,C27)+B27</f>
         <v>6173946.7274915744</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27" si="9">-PMT(A$11,A$5,D27)</f>
+        <f t="shared" ref="E27" si="14">-PMT(A$11,A$5,D27)</f>
         <v>826560.45590642723</v>
       </c>
       <c r="F27">
@@ -965,7 +1099,7 @@
         <v>1.1794527053459293E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>17</v>
       </c>
@@ -985,7 +1119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1141,7 @@
         <v>0.13085106382978723</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1021,15 +1155,15 @@
         <v>63</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" ref="E31:E34" si="10">(B31)/(D31*1000000*100)</f>
+        <f t="shared" ref="E31:E34" si="15">(B31)/(D31*1000000*100)</f>
         <v>0.43809523809523809</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" ref="F31:F33" si="11">(C31)/(D31*1000000*100)</f>
+        <f t="shared" ref="F31:F33" si="16">(C31)/(D31*1000000*100)</f>
         <v>0.14301587301587301</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1043,11 +1177,11 @@
         <v>294</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1065,11 +1199,11 @@
         <v>294</v>
       </c>
       <c r="E33" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.1598639455782313</v>
       </c>
       <c r="F33" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.11326530612244898</v>
       </c>
     </row>
@@ -1081,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="E34" s="3" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1095,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248186C2-819E-40A3-BDA6-AECDD5B5B57C}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7:Y7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
parameter values for sensitivty analysis
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/plant_costs.xlsx
+++ b/gcam/input/biochar_land_R/plant_costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B9AB2-B193-4427-9593-8929AD134FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A904AF-6BD1-4DA3-B2B0-A29EE78E49DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biochar_land" sheetId="2" r:id="rId1"/>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C229AC-139E-41F1-AA79-F61EE8EC5D09}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>